<commit_message>
Work In Progress: Refactor of input data
</commit_message>
<xml_diff>
--- a/pos_xref/data/raw/Incentive Comp - 2025.xlsx
+++ b/pos_xref/data/raw/Incentive Comp - 2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eddiec11us\Documents\vs code workspaces\PyLab\pos_xref\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eddiec11us\Documents\vs code workspaces\project_root\pos_xref\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048C0C2D-55CE-4DB2-ACDB-955CF5E216EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36E8438-9A45-4EA5-8F04-3D6C5603DD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5925" yWindow="3795" windowWidth="17910" windowHeight="15300" activeTab="2" xr2:uid="{DB937CF1-C7D7-4F2B-97D0-22CBE92A3C6B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{DB937CF1-C7D7-4F2B-97D0-22CBE92A3C6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Refresh Process" sheetId="4" r:id="rId1"/>
@@ -297,15 +297,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -313,20 +319,77 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="9"/>
+        </left>
+        <right style="thin">
+          <color theme="9"/>
+        </right>
+        <top style="thin">
+          <color theme="9"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -351,7 +414,7 @@
   <autoFilter ref="A4:I30" xr:uid="{A969B1B3-E0A3-4455-9CF5-8F7155CFDA32}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{40648AE7-7584-4692-A8AC-679CA74F8585}" name="Customer Name"/>
-    <tableColumn id="2" xr3:uid="{96A23410-E4DA-446B-B8C3-F60512585279}" name="Inventory ID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{96A23410-E4DA-446B-B8C3-F60512585279}" name="Inventory ID" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{42572DD2-76C4-4C9D-8609-AA31AEE54240}" name="Net Quantity"/>
     <tableColumn id="4" xr3:uid="{DF5C5F2E-953E-44EB-B37A-C207C18CBA6B}" name="Bill To Zip"/>
     <tableColumn id="5" xr3:uid="{458A7226-1513-482D-AF46-BC2F9F4B86E1}" name="Bill To St"/>
@@ -369,9 +432,9 @@
   <autoFilter ref="A6:H31" xr:uid="{E0390DE7-5F0F-46E3-9796-AF4CD7C776DC}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{5617EF9B-7554-49B0-BF8A-F9C4B2141239}" name="SoldToName"/>
-    <tableColumn id="2" xr3:uid="{75D0E5F8-7001-4C42-B39E-2CED27673A03}" name="PiiPartNumber" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{75D0E5F8-7001-4C42-B39E-2CED27673A03}" name="PiiPartNumber" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{47CEE127-2B19-45E8-8B6E-782342B8AF51}" name="ShipQty"/>
-    <tableColumn id="4" xr3:uid="{E916993E-F6EC-4971-A750-53146E178B3F}" name="BillToCustomerZip"/>
+    <tableColumn id="4" xr3:uid="{E916993E-F6EC-4971-A750-53146E178B3F}" name="BillToCustomerZip" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{10741991-6CBF-454D-B5FD-577E83E27448}" name="BillToCustomerState"/>
     <tableColumn id="6" xr3:uid="{47470273-0F9E-4697-B34F-2F43231D75C7}" name="Customer"/>
     <tableColumn id="7" xr3:uid="{7A65AF2E-BD9B-4CC7-AA8A-325CBA001015}" name="PiiCategory"/>
@@ -1214,7 +1277,7 @@
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -1267,11 +1330,11 @@
       <c r="C7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2">
+        <v>10001</v>
+      </c>
+      <c r="E7" t="s">
         <v>4</v>
-      </c>
-      <c r="E7">
-        <v>10001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1284,11 +1347,11 @@
       <c r="C8" s="1">
         <v>12</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3">
+        <v>90210</v>
+      </c>
+      <c r="E8" t="s">
         <v>7</v>
-      </c>
-      <c r="E8">
-        <v>90210</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1301,11 +1364,11 @@
       <c r="C9" s="1">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
         <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1318,11 +1381,11 @@
       <c r="C10" s="1">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3">
+        <v>950148854</v>
+      </c>
+      <c r="E10" t="s">
         <v>7</v>
-      </c>
-      <c r="E10">
-        <v>950148854</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1335,11 +1398,11 @@
       <c r="C11" s="1">
         <v>6</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
         <v>15</v>
-      </c>
-      <c r="E11" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1352,11 +1415,11 @@
       <c r="C12" s="1">
         <v>3</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
         <v>15</v>
-      </c>
-      <c r="E12" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1369,11 +1432,11 @@
       <c r="C13" s="1">
         <v>15</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2">
+        <v>60502</v>
+      </c>
+      <c r="E13" t="s">
         <v>21</v>
-      </c>
-      <c r="E13">
-        <v>60502</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1386,11 +1449,11 @@
       <c r="C14" s="1">
         <v>9</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3">
+        <v>60502</v>
+      </c>
+      <c r="E14" t="s">
         <v>21</v>
-      </c>
-      <c r="E14">
-        <v>60502</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1403,11 +1466,11 @@
       <c r="C15" s="1">
         <v>11</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2">
+        <v>73128</v>
+      </c>
+      <c r="E15" t="s">
         <v>26</v>
-      </c>
-      <c r="E15">
-        <v>73128</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1420,11 +1483,11 @@
       <c r="C16" s="1">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3">
+        <v>73128</v>
+      </c>
+      <c r="E16" t="s">
         <v>26</v>
-      </c>
-      <c r="E16">
-        <v>73128</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1437,11 +1500,11 @@
       <c r="C17">
         <v>12</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2">
+        <v>75201</v>
+      </c>
+      <c r="E17" t="s">
         <v>29</v>
-      </c>
-      <c r="E17">
-        <v>75201</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1454,11 +1517,11 @@
       <c r="C18">
         <v>13</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3">
+        <v>77001</v>
+      </c>
+      <c r="E18" t="s">
         <v>29</v>
-      </c>
-      <c r="E18">
-        <v>77001</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1471,11 +1534,11 @@
       <c r="C19">
         <v>8</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2">
+        <v>7097</v>
+      </c>
+      <c r="E19" t="s">
         <v>32</v>
-      </c>
-      <c r="E19">
-        <v>7097</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1488,11 +1551,11 @@
       <c r="C20">
         <v>4</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3">
+        <v>85001</v>
+      </c>
+      <c r="E20" t="s">
         <v>34</v>
-      </c>
-      <c r="E20">
-        <v>85001</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1505,11 +1568,11 @@
       <c r="C21">
         <v>4</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2">
+        <v>80202</v>
+      </c>
+      <c r="E21" t="s">
         <v>36</v>
-      </c>
-      <c r="E21">
-        <v>80202</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1522,11 +1585,11 @@
       <c r="C22">
         <v>2</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
         <v>38</v>
-      </c>
-      <c r="E22" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1539,11 +1602,11 @@
       <c r="C23">
         <v>20</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2">
+        <v>60601</v>
+      </c>
+      <c r="E23" t="s">
         <v>21</v>
-      </c>
-      <c r="E23">
-        <v>60601</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1556,11 +1619,11 @@
       <c r="C24">
         <v>19</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="3">
+        <v>98101</v>
+      </c>
+      <c r="E24" t="s">
         <v>42</v>
-      </c>
-      <c r="E24">
-        <v>98101</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1573,11 +1636,11 @@
       <c r="C25">
         <v>2</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2">
+        <v>33101</v>
+      </c>
+      <c r="E25" t="s">
         <v>44</v>
-      </c>
-      <c r="E25">
-        <v>33101</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1590,11 +1653,11 @@
       <c r="C26">
         <v>18</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="3">
+        <v>30301</v>
+      </c>
+      <c r="E26" t="s">
         <v>46</v>
-      </c>
-      <c r="E26">
-        <v>30301</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1607,11 +1670,11 @@
       <c r="C27">
         <v>8</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="2">
+        <v>27513</v>
+      </c>
+      <c r="E27" t="s">
         <v>48</v>
-      </c>
-      <c r="E27">
-        <v>27513</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1624,11 +1687,11 @@
       <c r="C28">
         <v>5</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="3">
+        <v>63101</v>
+      </c>
+      <c r="E28" t="s">
         <v>50</v>
-      </c>
-      <c r="E28">
-        <v>63101</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1641,11 +1704,11 @@
       <c r="C29">
         <v>15</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="2">
+        <v>48201</v>
+      </c>
+      <c r="E29" t="s">
         <v>52</v>
-      </c>
-      <c r="E29">
-        <v>48201</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1658,11 +1721,11 @@
       <c r="C30">
         <v>11</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="3">
+        <v>11201</v>
+      </c>
+      <c r="E30" t="s">
         <v>4</v>
-      </c>
-      <c r="E30">
-        <v>11201</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1675,11 +1738,11 @@
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="2">
+        <v>95814</v>
+      </c>
+      <c r="E31" t="s">
         <v>7</v>
-      </c>
-      <c r="E31">
-        <v>95814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>